<commit_message>
Version inicial del proyecto
</commit_message>
<xml_diff>
--- a/contratos_lab.xlsx
+++ b/contratos_lab.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,11 @@
           <t>contract_date</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>estimated_end_date</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -664,11 +669,12 @@
         </is>
       </c>
       <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0010p</t>
+          <t>Prueba099</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -694,73 +700,73 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Andrés Felipe Cadavid</t>
+          <t>PEPE2 PRUEBA PRUEBA</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>7888888</v>
+        <v>2222222</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Pinar de Canada</t>
+          <t>DIRECCION PRUEBA</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Medellin Ant.</t>
+          <t>Medellín PRUEBA</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>1999-10-05</t>
+          <t>1998-08-08</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>3005559999</v>
+        <v>30234445</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>prueba15@gmail.com</t>
+          <t>PRUEBA@CORREO.COM</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>María Alejandra Pineda, 3007775544</t>
+          <t>31111111</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Ayudante de Obra</t>
+          <t>OFICIAL DE OBRA PRUEBA</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2025-07-17</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Actividades de Construcción</t>
+          <t>actividades de prueba quince</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>30%  avance de obra del proyecto</t>
+          <t>30% Avance de obra del proyecto PRUEBA</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Proyecto EBANO</t>
+          <t>Proyecto PRUEBA</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Rionegro</t>
+          <t>Medellín PRUEBA</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>DOS MILLONES DE PESOS COLOMBIANOS ($2.000.000)</t>
+          <t>DOS MILLONES CIEN MIL PESOS COLOMBIANOS ($2.100.000)</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -775,14 +781,19 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>2025-12-19</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0011p</t>
+          <t>005Prueba</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -808,78 +819,78 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Andrés Felipe Bermúdez</t>
+          <t>PEDRO4 PRUEBA</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>15389120</v>
+        <v>2222222</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Carrera 43E #6-51 Rionegro Antioquia</t>
+          <t>DIRECCION PRUEBA</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Medellín Antioquia</t>
+          <t>Medellín PRUEBA</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1999-10-05</t>
+          <t>1998-08-08</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>3005559999</v>
+        <v>30234445</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>prueba15@gmail.com</t>
+          <t>PRUEBA@CORREO.COM</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>María Alejandra Pineda, 300777554</t>
+          <t>31111111</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Ayudante Eelectrico</t>
+          <t>OFICIAL DE OBRA PRUEBA</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2025-07-17</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Actividades eléctricas, de energía, técnicas, de construcción y demás relacionadas</t>
+          <t>actividades de prueba</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>30% avance de la torre 2, sub etapa 1</t>
+          <t>30% Avance de obra del proyecto PRUEBA</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Proyecto BOSQUE BOREAL</t>
+          <t>Proyecto PRUEBA</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Carmen de Viboral, Antioquia.</t>
+          <t>Medellín PRUEBA</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>DOS MILLONES QUINIENTOS MIL PESOS COLOMBIANOS ($2.500.000)</t>
+          <t>DOS MILLONES CIEN MIL PESOS COLOMBIANOS ($2.100.000)</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Quincenal</t>
+          <t>Mensual</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -889,25 +900,28 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>2025-07-10</t>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>2025-12-19</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>01-1211</t>
+          <t>0016PRUEBA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ROMBO ESCARLATA SAS</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>900902510-0</t>
-        </is>
+          <t>INGEURBANISMO SAS</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>900474198</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -924,78 +938,78 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>JORGE LUIS MADRID CAMPOS</t>
+          <t>ROBERTO PRUEBA PRUEBA</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1127218432</v>
+        <v>11111117</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Carrera 43E #6-51 Rionegro Antioquia</t>
+          <t>DIRECCION PRUEBA</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Medellín Antioquia</t>
+          <t>Medellín PRUEBA</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1974-03-31</t>
+          <t>1990-02-17</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3023806465</v>
+        <v>30234445</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>SIN@CORREO.COM</t>
+          <t>PRUEBA@CORREO.COM</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>GUILLERMO LUNA, 3002623499</t>
+          <t>María prueba prueba</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t xml:space="preserve">AYUDANTE DE OBRA </t>
+          <t>OFICIAL DE OBRA PRUEBA</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACTIVIDADES DE OBRA RELACIONADAS A LA VIA EXTERNA </t>
+          <t>Pilotes</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t xml:space="preserve">80% SEGUN AVANCE DE OBRA DE LA VIA EXTERNA </t>
+          <t>50% Avance de obra del proyecto PRUEBA</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Proyecto BOSQUE BOREAL</t>
+          <t>Proyecto PRUEBA</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Carmen de Viboral, Antioquia.</t>
+          <t>Medellín PRUEBA</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>UN MILLON CUATROSCIENTOS VEINTITRES MIL QUINIENTOS PESOS M/C ($1.423.500)</t>
+          <t>DOS MILLONES CIEN MIL PESOS COLOMBIANOS ($2.100.000)</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Quincenal</t>
+          <t>Mensual</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1005,14 +1019,19 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>2025-06-16</t>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01-1496</t>
+          <t>Prueba2D</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1020,116 +1039,351 @@
           <t>INGEURBANISMO SAS</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>900474198</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ELIANA MARIA ARBELAEZ ALZATE</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1038407657</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Km 4, Vía Llanogrande - Don Diego</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>David Prueba Prueba2</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>11111118</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>DIRECCION PRUEBA</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Medellín PRUEBA</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1990-02-17</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>30234445</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>PRUEBA@CORREO.COM</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>María prueba prueba</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>OFICIAL DE OBRA PRUEBA</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>actividades de prueba</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>50% Avance de obra del proyecto PRUEBA</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Proyecto PRUEBA</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Medellín PRUEBA</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>DOS MILLONES CIEN MIL PESOS COLOMBIANOS ($2.100.000)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Obra o Labor</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>2025-09-21</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Prueba3m</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>INGEURBANISMO SAS</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>900474198</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ELIANA MARIA ARBELAEZ ALZATE</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1038407657</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Km 4, Vía Llanogrande - Don Diego</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>LUIS PRUEBA3</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>11111118</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>DIRECCION PRUEBA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Medellín PRUEBA</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1990-02-17</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>30234445</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>PRUEBA@CORREO.COM</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>JOSE PRUEBA3</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>OFICIAL DE OBRA PRUEBA</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>actividades de prueba</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>50% Avance de obra del proyecto PRUEBA</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Proyecto PRUEBA</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Medellín PRUEBA</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>DOS MILLONES CIEN MIL PESOS COLOMBIANOS ($2.100.000)</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Obra o Labor</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>2025-09-21</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>00PTI</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>INGEURBANISMO SAS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>900474198</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>ELIANA MARIA ARBELAEZ ALZATE</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>1038407657</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Km 4, Vía Llanogrande - Don Diego</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>JUAN CAMILO HOLGUIN CORREAL</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1020411970</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>DIAGONAL 61 #48 E 08</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Medellin Ant.</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>1988-02-21</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>3023162214</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>SIN@CORREO.COM</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Javier Vargas</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OFICIAL DE OBRA </t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>2025-06-17</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Actividades de construcción y eléctricas.</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>90% segun avance de obra del proyecto</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Proyecto NUBARA</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Medellin Ant.</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>DOS MILLONES CIEN MIL PESOS COLOMBIANOS ($2.100.000)</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Quincenal</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>Obra o Labor</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>2025-06-15</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Prueba 5</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Rionegro</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>CR 17 A NRO. 20 20 , La Ceja</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>La Ceja</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1990-10-12</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2222222</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>fachadas.abs22@gmail.com</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>LAURA PRUEBA PRUEBA</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Contador</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Líder del Área Contable</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>INGEURBANISMO SAS</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Rionegro, Antioquia.</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>CUATRO MILLONES DE PESOS ($4.000.000)</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Término Indefinido</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>